<commit_message>
Added limits to the arm based on angle limits
</commit_message>
<xml_diff>
--- a/TeamCode/src/main/java/org/firstinspires/ftc/teamcode/robot/test/Arm Angles.xlsx
+++ b/TeamCode/src/main/java/org/firstinspires/ftc/teamcode/robot/test/Arm Angles.xlsx
@@ -5,29 +5,35 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joelm\Desktop\Personal\IHS Robotics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joelm\Desktop\Personal\FTC-2019\TeamCode\src\main\java\org\firstinspires\ftc\teamcode\robot\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A14A435-C0CC-4A93-A2BA-541AD4A8BF00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C151BBCB-EE3B-4CC1-AAA1-E029541C327E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{BA1C8E53-012E-4F44-9ED0-51D2C78C7643}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{BA1C8E53-012E-4F44-9ED0-51D2C78C7643}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Motor Commands" sheetId="2" r:id="rId2"/>
+    <sheet name="Arm Controls" sheetId="1" r:id="rId1"/>
+    <sheet name="Claw" sheetId="3" r:id="rId2"/>
+    <sheet name="Claw Vertical" sheetId="4" r:id="rId3"/>
+    <sheet name="Motor Commands" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="A">Sheet1!$B$11</definedName>
-    <definedName name="b_ang">Sheet1!$B$10</definedName>
-    <definedName name="HYPOT">Sheet1!$B$8</definedName>
-    <definedName name="LOWER_LENGTH">Sheet1!$B$6</definedName>
-    <definedName name="M">Sheet1!$B$12</definedName>
-    <definedName name="N">Sheet1!$B$9</definedName>
-    <definedName name="S1_">Sheet1!$B$4</definedName>
-    <definedName name="S2_">Sheet1!$B$5</definedName>
-    <definedName name="UPPER_LENGTH">Sheet1!$B$7</definedName>
-    <definedName name="x">Sheet1!$B$2</definedName>
-    <definedName name="y">Sheet1!$B$3</definedName>
+    <definedName name="A">'Arm Controls'!$B$11</definedName>
+    <definedName name="b_ang">'Arm Controls'!$B$10</definedName>
+    <definedName name="HYPOT">'Arm Controls'!$B$8</definedName>
+    <definedName name="Lower_Arm_End_X">'Arm Controls'!$B$17</definedName>
+    <definedName name="Lower_Arm_End_Y">'Arm Controls'!$C$17</definedName>
+    <definedName name="LOWER_LENGTH">'Arm Controls'!$B$6</definedName>
+    <definedName name="M">'Arm Controls'!$B$12</definedName>
+    <definedName name="N">'Arm Controls'!$B$9</definedName>
+    <definedName name="S1_">'Arm Controls'!$B$4</definedName>
+    <definedName name="S2_">'Arm Controls'!$B$5</definedName>
+    <definedName name="Upper_Arm_End_X">'Arm Controls'!$D$17</definedName>
+    <definedName name="Upper_Arm_End_Y">'Arm Controls'!$E$17</definedName>
+    <definedName name="UPPER_LENGTH">'Arm Controls'!$B$7</definedName>
+    <definedName name="x">'Arm Controls'!$B$2</definedName>
+    <definedName name="y">'Arm Controls'!$B$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="77">
   <si>
     <t>Parameter</t>
   </si>
@@ -182,13 +188,100 @@
     <t>Output</t>
   </si>
   <si>
-    <t>Claw X</t>
-  </si>
-  <si>
-    <t>Claw Y</t>
-  </si>
-  <si>
     <t>Claw Dimensions</t>
+  </si>
+  <si>
+    <t>Rotation Joint</t>
+  </si>
+  <si>
+    <t>Top Right of Servo</t>
+  </si>
+  <si>
+    <t>Top Left of Servo</t>
+  </si>
+  <si>
+    <t>Bottom Right of Servo</t>
+  </si>
+  <si>
+    <t>Bottom Left of Servo</t>
+  </si>
+  <si>
+    <t>Arm Joint</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Rotation Servo</t>
+  </si>
+  <si>
+    <t>Offset Y</t>
+  </si>
+  <si>
+    <t>Offset X</t>
+  </si>
+  <si>
+    <t>Width</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Claw</t>
+  </si>
+  <si>
+    <t>Claw Holder</t>
+  </si>
+  <si>
+    <t>Relative To</t>
+  </si>
+  <si>
+    <t>Claw Holder BL</t>
+  </si>
+  <si>
+    <t>Claw Holder BR</t>
+  </si>
+  <si>
+    <t>Claw Holder TR</t>
+  </si>
+  <si>
+    <t>Claw Holder TL</t>
+  </si>
+  <si>
+    <t>Claw BL</t>
+  </si>
+  <si>
+    <t>Claw BR</t>
+  </si>
+  <si>
+    <t>Claw TL</t>
+  </si>
+  <si>
+    <t>Claw TR</t>
+  </si>
+  <si>
+    <t>A Joint</t>
+  </si>
+  <si>
+    <t>Rotation of Servo</t>
+  </si>
+  <si>
+    <t>Upper Arm Slope</t>
+  </si>
+  <si>
+    <t>y = mx + b</t>
+  </si>
+  <si>
+    <t>b = y - m*x</t>
+  </si>
+  <si>
+    <t>X value at top of claw</t>
+  </si>
+  <si>
+    <t>x = (y-b)/m</t>
   </si>
 </sst>
 </file>
@@ -283,7 +376,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$16:$B$17</c:f>
+              <c:f>'Arm Controls'!$B$16:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -291,14 +384,14 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-5.4080504577458353</c:v>
+                  <c:v>-2.2302857878969564</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$16:$C$17</c:f>
+              <c:f>'Arm Controls'!$C$16:$C$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -306,7 +399,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.408050457745839</c:v>
+                  <c:v>12.426441578517352</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -338,30 +431,30 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$D$16:$D$17</c:f>
+              <c:f>'Arm Controls'!$D$16:$D$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>-5.4080504577458353</c:v>
+                  <c:v>-2.2302857878969564</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.0000000000000018</c:v>
+                  <c:v>6.0000000000000071</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$16:$E$17</c:f>
+              <c:f>'Arm Controls'!$E$16:$E$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>11.408050457745839</c:v>
+                  <c:v>12.426441578517352</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.9999999999999964</c:v>
+                  <c:v>21.999999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -370,116 +463,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-EA5F-4024-9550-7CBDCE30F8B4}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>Claw X</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$F$16:$F$17</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>6.0000000000000018</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9.3750000000000018</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$G$16:$G$17</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>5.9999999999999964</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.9999999999999964</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-BC71-4257-952A-7FFEC7A346EA}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:v>Claw Y</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$H$16:$H$17</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>9.3750000000000018</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9.3750000000000018</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$I$16:$I$17</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>5.9999999999999964</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.99999999999999645</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-BC71-4257-952A-7FFEC7A346EA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -676,6 +659,1228 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Right of Servo</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(Claw!$B$12,Claw!$B$14)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>9.0000000000000071</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.0000000000000071</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(Claw!$C$12,Claw!$C$14)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>19.749999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22.499999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-03AB-4BE1-AA36-94FF36C2FA1A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Left of Servo</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(Claw!$B$11,Claw!$B$13)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>6.5000000000000071</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.5000000000000071</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(Claw!$C$11,Claw!$C$13)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>19.749999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22.499999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-03AB-4BE1-AA36-94FF36C2FA1A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Top of Servo</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Claw!$B$13:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>6.5000000000000071</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.0000000000000071</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Claw!$C$13:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>22.499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22.499999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-03AB-4BE1-AA36-94FF36C2FA1A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Bottom of Servo</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Claw!$B$11:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>6.5000000000000071</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.0000000000000071</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Claw!$C$11:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>19.749999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19.749999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-03AB-4BE1-AA36-94FF36C2FA1A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Arm Joint</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Claw!$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>6.0000000000000071</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Claw!$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>21.999999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-03AB-4BE1-AA36-94FF36C2FA1A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>Rotation Joint</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Claw!$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>7.0000000000000071</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Claw!$C$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>19.499999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-03AB-4BE1-AA36-94FF36C2FA1A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>Claw Holder Left</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(Claw!$B$16,Claw!$B$18)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>7.0000000000000071</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.0000000000000071</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(Claw!$C$16,Claw!$C$18)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>19.249999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19.499999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-03AB-4BE1-AA36-94FF36C2FA1A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:v>Claw Holder Right</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(Claw!$B$17,Claw!$B$19)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>10.500000000000007</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.500000000000007</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(Claw!$C$17,Claw!$C$19)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>19.249999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19.499999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-03AB-4BE1-AA36-94FF36C2FA1A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:v>Claw Holder Top</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Claw!$B$18:$B$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>7.0000000000000071</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.500000000000007</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Claw!$C$18:$C$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>19.499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19.499999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-03AB-4BE1-AA36-94FF36C2FA1A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:v>Claw Holder Bottom</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Claw!$B$16:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>7.0000000000000071</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.500000000000007</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Claw!$C$16:$C$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>19.249999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19.249999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-03AB-4BE1-AA36-94FF36C2FA1A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:v>Claw Left</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(Claw!$B$20,Claw!$B$22)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>8.1250000000000071</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.1250000000000071</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(Claw!$C$20,Claw!$C$22)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>14.249999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19.249999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-03AB-4BE1-AA36-94FF36C2FA1A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="11"/>
+          <c:tx>
+            <c:v>Claw Right</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(Claw!$B$21,Claw!$B$23)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>11.625000000000007</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.625000000000007</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(Claw!$C$21,Claw!$C$23)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>14.249999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19.249999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000D-03AB-4BE1-AA36-94FF36C2FA1A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="12"/>
+          <c:order val="12"/>
+          <c:tx>
+            <c:v>Claw Top</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Claw!$B$22:$B$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>8.1250000000000071</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.625000000000007</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Claw!$C$22:$C$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>19.249999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19.249999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000E-03AB-4BE1-AA36-94FF36C2FA1A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="13"/>
+          <c:order val="13"/>
+          <c:tx>
+            <c:v>Lower Arm</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Claw!$B$24:$B$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>-2.2302857878969564</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Claw!$C$24:$C$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>12.426441578517352</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000F-03AB-4BE1-AA36-94FF36C2FA1A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="14"/>
+          <c:order val="14"/>
+          <c:tx>
+            <c:v>Upper Arm</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(Claw!$B$10,Claw!$B$24)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>6.0000000000000071</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-2.2302857878969564</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(Claw!$C$10,Claw!$C$24)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>21.999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.426441578517352</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000010-03AB-4BE1-AA36-94FF36C2FA1A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="15"/>
+          <c:order val="15"/>
+          <c:tx>
+            <c:v>X at Claw</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="80000"/>
+                    <a:lumOff val="20000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Claw!$H$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3.6358544106307971</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Claw!$C$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>19.249999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000011-03AB-4BE1-AA36-94FF36C2FA1A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="16"/>
+          <c:order val="16"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Claw!$H$10:$H$14</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3.635854411</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.429844653</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.570155347</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.710466042</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.017825137</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Claw!$H$10:$H$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3.6358544106307971</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.4298446526125943</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.570155347387427</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.7104660421622597</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-1.7825136576160701E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Claw!$I$10:$I$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>19.249999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000012-03AB-4BE1-AA36-94FF36C2FA1A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1362398975"/>
+        <c:axId val="1363969711"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1362398975"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1363969711"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1363969711"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1362398975"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1172,6 +2377,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1689,6 +2934,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2246,6 +4007,47 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>160020</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7317916-BCD5-4BA4-BB3F-1B0C4BB351DB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2585,8 +4387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECC4DB7A-D314-417E-B4DA-F69266E375DE}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2652,7 +4454,7 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -2676,7 +4478,7 @@
       </c>
       <c r="B4">
         <f>b_ang+N</f>
-        <v>115.36355397794352</v>
+        <v>100.17505896230035</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
@@ -2693,8 +4495,8 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <f>A-M</f>
-        <v>64.636446022056447</v>
+        <f>MAX(A-M,$H$8)</f>
+        <v>139.31470363158405</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
@@ -2740,7 +4542,7 @@
       </c>
       <c r="B8">
         <f>SQRT(x^2+y^2)</f>
-        <v>8.4852813742385695</v>
+        <v>22.803508501982758</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
@@ -2764,7 +4566,7 @@
       </c>
       <c r="B9">
         <f>DEGREES(ATAN2(x,y))</f>
-        <v>45</v>
+        <v>74.744881296942225</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
@@ -2779,7 +4581,7 @@
       </c>
       <c r="B10">
         <f>DEGREES(ACOS((UPPER_LENGTH^2-LOWER_LENGTH^2-HYPOT^2)/(-2*LOWER_LENGTH*HYPOT)))</f>
-        <v>70.363553977943525</v>
+        <v>25.43017766535813</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
@@ -2793,8 +4595,8 @@
         <v>25</v>
       </c>
       <c r="B11">
-        <f>DEGREES(ACOS((HYPOT^2-UPPER_LENGTH^2-LOWER_LENGTH^2)/(-2*UPPER_LENGTH*LOWER_LENGTH)))</f>
-        <v>39.272892044112929</v>
+        <f>MAX(DEGREES(ACOS((HYPOT^2-UPPER_LENGTH^2-LOWER_LENGTH^2)/(-2*UPPER_LENGTH*LOWER_LENGTH))),$H$8)</f>
+        <v>129.13964466928371</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
@@ -2809,7 +4611,7 @@
       </c>
       <c r="B12">
         <f>90-S1_</f>
-        <v>-25.363553977943525</v>
+        <v>-10.175058962300355</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
@@ -2834,18 +4636,6 @@
       <c r="E15" t="s">
         <v>30</v>
       </c>
-      <c r="F15" t="s">
-        <v>45</v>
-      </c>
-      <c r="G15" t="s">
-        <v>45</v>
-      </c>
-      <c r="H15" t="s">
-        <v>46</v>
-      </c>
-      <c r="I15" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
@@ -2861,88 +4651,56 @@
       </c>
       <c r="D16">
         <f>UPPER_LENGTH*COS(RADIANS(S2_-90))*A16+$B$17</f>
-        <v>-5.4080504577458353</v>
+        <v>-2.2302857878969564</v>
       </c>
       <c r="E16">
         <f>UPPER_LENGTH*SIN(RADIANS(S2_-90))*A16+$C$17</f>
-        <v>11.408050457745839</v>
-      </c>
-      <c r="F16">
-        <f>D17</f>
-        <v>6.0000000000000018</v>
-      </c>
-      <c r="G16">
-        <f>E17</f>
-        <v>5.9999999999999964</v>
-      </c>
-      <c r="H16">
-        <f>F17</f>
-        <v>9.3750000000000018</v>
-      </c>
-      <c r="I16">
-        <f>G17</f>
-        <v>5.9999999999999964</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+        <v>12.426441578517352</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1</v>
       </c>
       <c r="B17">
         <f>LOWER_LENGTH*COS(RADIANS(S1_))*A17</f>
-        <v>-5.4080504577458353</v>
+        <v>-2.2302857878969564</v>
       </c>
       <c r="C17">
         <f>LOWER_LENGTH*SIN(RADIANS(S1_))*A17</f>
-        <v>11.408050457745839</v>
+        <v>12.426441578517352</v>
       </c>
       <c r="D17">
         <f>UPPER_LENGTH*COS(RADIANS(S2_-90))*A17+$B$17</f>
-        <v>6.0000000000000018</v>
+        <v>6.0000000000000071</v>
       </c>
       <c r="E17">
         <f>UPPER_LENGTH*SIN(RADIANS(S2_-90))*A17+$C$17</f>
-        <v>5.9999999999999964</v>
-      </c>
-      <c r="F17">
-        <f>F16+$F$24</f>
-        <v>9.3750000000000018</v>
-      </c>
-      <c r="G17">
-        <f>G16</f>
-        <v>5.9999999999999964</v>
-      </c>
-      <c r="H17">
-        <f>H16</f>
-        <v>9.3750000000000018</v>
-      </c>
-      <c r="I17">
-        <f>I16-$F$25</f>
-        <v>0.99999999999999645</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+        <v>21.999999999999996</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>31</v>
       </c>
       <c r="B19">
         <f>B17-B16</f>
-        <v>-5.4080504577458353</v>
+        <v>-2.2302857878969564</v>
       </c>
       <c r="C19">
         <f>C17-C16</f>
-        <v>11.408050457745839</v>
+        <v>12.426441578517352</v>
       </c>
       <c r="D19">
         <f>D17-D16</f>
-        <v>11.408050457745837</v>
+        <v>8.230285787896964</v>
       </c>
       <c r="E19">
         <f>E17-E16</f>
-        <v>-5.4080504577458424</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+        <v>9.5735584214826446</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -2952,19 +4710,19 @@
       </c>
       <c r="D20">
         <f>SQRT(D19*D19+E19*E19)</f>
-        <v>12.625000000000002</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+        <v>12.625</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>40</v>
       </c>
       <c r="B22">
         <f>SQRT(SUMSQ(B2:B3))</f>
-        <v>8.4852813742385695</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+        <v>22.803508501982758</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -2973,10 +4731,10 @@
         <v>25.25</v>
       </c>
       <c r="E23" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -2991,7 +4749,7 @@
         <v>3.375</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -3013,10 +4771,521 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E09FCC97-4F6C-4DBA-BB11-DBBC64DD5AA1}">
+  <dimension ref="A1:I25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="A1:F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2">
+        <v>2.5</v>
+      </c>
+      <c r="C2">
+        <v>2.75</v>
+      </c>
+      <c r="D2">
+        <v>0.5</v>
+      </c>
+      <c r="E2">
+        <v>0.5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2">
+        <f>(Upper_Arm_End_Y-Lower_Arm_End_Y)/(Upper_Arm_End_X-Lower_Arm_End_X)</f>
+        <v>1.1632109343713226</v>
+      </c>
+      <c r="I2">
+        <f>(Upper_Arm_End_Y-Lower_Arm_End_Y)/(Upper_Arm_End_X-Lower_Arm_End_X)</f>
+        <v>1.1632109343713226</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>-2.5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4">
+        <f>3.5*COS(RADIANS($B$6))</f>
+        <v>3.5</v>
+      </c>
+      <c r="C4">
+        <v>0.25</v>
+      </c>
+      <c r="F4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5">
+        <f>4.75*COS(RADIANS($B$6))</f>
+        <v>4.75</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <f>D3</f>
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <f>E3-0.5</f>
+        <v>-3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5">
+        <f>C10-H2*B10</f>
+        <v>15.020734393772052</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" t="s">
+        <v>52</v>
+      </c>
+      <c r="H9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10">
+        <f>'Arm Controls'!D17</f>
+        <v>6.0000000000000071</v>
+      </c>
+      <c r="C10">
+        <f>'Arm Controls'!E17</f>
+        <v>21.999999999999996</v>
+      </c>
+      <c r="H10">
+        <f>(I10-$H$5)/$H$2</f>
+        <v>3.6358544106307971</v>
+      </c>
+      <c r="I10">
+        <f>C22</f>
+        <v>19.249999999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11">
+        <f>$B$10+$D$2</f>
+        <v>6.5000000000000071</v>
+      </c>
+      <c r="C11">
+        <f>$C$10+$E$2-$C$2</f>
+        <v>19.749999999999996</v>
+      </c>
+      <c r="H11">
+        <f>(I11-$H$5)/$H$2</f>
+        <v>6.4298446526125943</v>
+      </c>
+      <c r="I11">
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12">
+        <f>$B$10+$D$2+$B$2</f>
+        <v>9.0000000000000071</v>
+      </c>
+      <c r="C12">
+        <f>$C$10+$E$2-$C$2</f>
+        <v>19.749999999999996</v>
+      </c>
+      <c r="H12">
+        <f>(I12-$H$5)/$H$2</f>
+        <v>5.570155347387427</v>
+      </c>
+      <c r="I12">
+        <f>I11-1</f>
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13">
+        <f>$B$10+$D$2</f>
+        <v>6.5000000000000071</v>
+      </c>
+      <c r="C13">
+        <f>$C$10+$E$2</f>
+        <v>22.499999999999996</v>
+      </c>
+      <c r="H13">
+        <f>(I13-$H$5)/$H$2</f>
+        <v>4.7104660421622597</v>
+      </c>
+      <c r="I13">
+        <f>I12-1</f>
+        <v>20.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14">
+        <f>$B$10+$D$2+$B$2</f>
+        <v>9.0000000000000071</v>
+      </c>
+      <c r="C14">
+        <f>$C$10+$E$2</f>
+        <v>22.499999999999996</v>
+      </c>
+      <c r="H14">
+        <f>(I14-$H$5)/$H$2</f>
+        <v>-1.7825136576160701E-2</v>
+      </c>
+      <c r="I14">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15">
+        <f>$B$10+$D$3</f>
+        <v>7.0000000000000071</v>
+      </c>
+      <c r="C15">
+        <f>$C$10+$E$3</f>
+        <v>19.499999999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16">
+        <f>B15</f>
+        <v>7.0000000000000071</v>
+      </c>
+      <c r="C16">
+        <f>C15-$C$4</f>
+        <v>19.249999999999996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17">
+        <f>B16+B4</f>
+        <v>10.500000000000007</v>
+      </c>
+      <c r="C17">
+        <f>C16</f>
+        <v>19.249999999999996</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18">
+        <f>B16</f>
+        <v>7.0000000000000071</v>
+      </c>
+      <c r="C18">
+        <f>C15</f>
+        <v>19.499999999999996</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19">
+        <f>B17</f>
+        <v>10.500000000000007</v>
+      </c>
+      <c r="C19">
+        <f>C15</f>
+        <v>19.499999999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20">
+        <f>$B$17-$B$5/2</f>
+        <v>8.1250000000000071</v>
+      </c>
+      <c r="C20">
+        <f>C16-$C$5</f>
+        <v>14.249999999999996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21">
+        <f>B20+$B$4</f>
+        <v>11.625000000000007</v>
+      </c>
+      <c r="C21">
+        <f>C17-$C$5</f>
+        <v>14.249999999999996</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22">
+        <f>$B$17-$B$5/2</f>
+        <v>8.1250000000000071</v>
+      </c>
+      <c r="C22">
+        <f>C17</f>
+        <v>19.249999999999996</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23">
+        <f>B22+$B$4</f>
+        <v>11.625000000000007</v>
+      </c>
+      <c r="C23">
+        <f>C17</f>
+        <v>19.249999999999996</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24">
+        <f>'Arm Controls'!D16</f>
+        <v>-2.2302857878969564</v>
+      </c>
+      <c r="C24">
+        <f>'Arm Controls'!E16</f>
+        <v>12.426441578517352</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{792E1F17-EE73-43F0-AF52-F5F0446CD6B5}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>-2.5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <f>3.5*COS(RADIANS($B$6))</f>
+        <v>3.5</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <f>4.75*COS(RADIANS($B$6))</f>
+        <v>4.75</v>
+      </c>
+      <c r="D5">
+        <f>D3</f>
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <f>E3-0.5</f>
+        <v>-3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE17A856-6ADF-448A-B7BD-69911367D557}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>